<commit_message>
feat: Excel Dateien erweitert
</commit_message>
<xml_diff>
--- a/Excel/Quantitative Analyse.xlsx
+++ b/Excel/Quantitative Analyse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11102"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/Thesis/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CAA0ECC4-1A6A-4533-B338-2544E1A9EF33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56C76D2-B746-5A4B-970B-AE29C2E1C97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Harmonisierung" sheetId="1" r:id="rId1"/>
@@ -395,6 +395,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -408,6 +409,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -421,6 +423,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -434,6 +437,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -447,6 +451,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -469,6 +474,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -491,6 +497,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -513,6 +520,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -535,6 +543,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -557,6 +566,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -579,6 +589,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -601,6 +612,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -623,6 +635,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -645,6 +658,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -667,6 +681,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -689,6 +704,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -711,6 +727,7 @@
         <sz val="11"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t> </t>
     </r>
@@ -781,11 +798,13 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -935,7 +954,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -960,7 +979,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -972,13 +991,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2270,6 +2286,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2277,7 +2294,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2616,6 +2632,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2623,7 +2640,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3364,6 +3380,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3371,7 +3388,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -6981,14 +6997,14 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.26953125" customWidth="1"/>
-    <col min="2" max="2" width="56.08984375" customWidth="1"/>
-    <col min="3" max="27" width="29.7265625" customWidth="1"/>
+    <col min="1" max="1" width="52.33203125" customWidth="1"/>
+    <col min="2" max="2" width="56.1640625" customWidth="1"/>
+    <col min="3" max="27" width="29.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>39</v>
       </c>
@@ -6996,7 +7012,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>33</v>
       </c>
@@ -7004,7 +7020,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
@@ -7012,7 +7028,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>28</v>
       </c>
@@ -7020,7 +7036,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>26</v>
       </c>
@@ -7028,7 +7044,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -7036,7 +7052,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -7044,7 +7060,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -7052,7 +7068,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>15</v>
       </c>
@@ -7060,7 +7076,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>14</v>
       </c>
@@ -7068,7 +7084,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -7076,7 +7092,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -7086,6 +7102,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -7099,156 +7116,157 @@
       <selection pane="bottomLeft" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.90625" customWidth="1"/>
-    <col min="2" max="3" width="21.453125" customWidth="1"/>
-    <col min="4" max="4" width="25.08984375" customWidth="1"/>
-    <col min="5" max="5" width="27.6328125" customWidth="1"/>
-    <col min="6" max="7" width="21.453125" customWidth="1"/>
-    <col min="8" max="8" width="27.6328125" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" customWidth="1"/>
+    <col min="2" max="3" width="21.5" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" customWidth="1"/>
+    <col min="5" max="5" width="27.6640625" customWidth="1"/>
+    <col min="6" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="24" t="s">
+      <c r="C1" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="F1" s="20"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="21">
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="20">
         <v>2021</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="18">
         <v>2</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="22"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="21">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="20">
         <v>2022</v>
       </c>
-      <c r="B3" s="19">
+      <c r="B3" s="18">
         <v>1</v>
       </c>
-      <c r="C3" s="19"/>
-      <c r="D3" s="17"/>
-      <c r="E3" s="22"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="21">
+      <c r="C3" s="18"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="20">
         <v>2023</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="18">
         <v>2</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="2"/>
-      <c r="E4" s="22"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="21">
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="20">
         <v>2024</v>
       </c>
-      <c r="B5" s="19">
+      <c r="B5" s="18">
         <v>5</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="18">
         <v>1</v>
       </c>
       <c r="D5" s="2">
         <v>1</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="26">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="25">
         <v>2025</v>
       </c>
-      <c r="B6" s="27">
+      <c r="B6" s="26">
         <v>6</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="26">
         <v>1</v>
       </c>
-      <c r="D6" s="28">
+      <c r="D6" s="27">
         <v>1</v>
       </c>
-      <c r="E6" s="29"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="18"/>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="18"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="18"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="18"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="18"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="18"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="18"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="18"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="18"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="18"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="18"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -7264,15 +7282,15 @@
       <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.26953125" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
-    <col min="3" max="3" width="37.81640625" customWidth="1"/>
-    <col min="5" max="6" width="23.1796875" style="31" customWidth="1"/>
+    <col min="1" max="1" width="31.33203125" customWidth="1"/>
+    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="3" max="3" width="37.83203125" customWidth="1"/>
+    <col min="5" max="6" width="23.1640625" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="11" t="s">
         <v>36</v>
       </c>
@@ -7282,14 +7300,14 @@
       <c r="C1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="34" t="s">
+      <c r="E1" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="F1" s="34" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>41</v>
       </c>
@@ -7299,14 +7317,14 @@
       <c r="C2" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="33">
+      <c r="F2" s="32">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
         <v>42</v>
       </c>
@@ -7316,14 +7334,14 @@
       <c r="C3" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="33">
+      <c r="F3" s="32">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="12" t="s">
         <v>43</v>
       </c>
@@ -7333,14 +7351,14 @@
       <c r="C4" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="31" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="33">
+      <c r="F4" s="32">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="12" t="s">
         <v>99</v>
       </c>
@@ -7350,14 +7368,14 @@
       <c r="C5" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="F5" s="33">
+      <c r="F5" s="32">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>100</v>
       </c>
@@ -7367,14 +7385,14 @@
       <c r="C6" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="F6" s="37">
+      <c r="F6" s="36">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>77</v>
       </c>
@@ -7384,14 +7402,14 @@
       <c r="C10" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="F10" s="40" t="s">
+      <c r="F10" s="39" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>80</v>
       </c>
@@ -7399,15 +7417,15 @@
         <v>85</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="E11" s="38" t="s">
+      <c r="E11" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="F11" s="42">
+      <c r="F11" s="41">
         <f xml:space="preserve"> 21/21</f>
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>81</v>
       </c>
@@ -7417,15 +7435,15 @@
       <c r="C12" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="38" t="s">
+      <c r="E12" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="42">
+      <c r="F12" s="41">
         <f xml:space="preserve"> 19/21</f>
         <v>0.90476190476190477</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>82</v>
       </c>
@@ -7435,15 +7453,15 @@
       <c r="C13" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="37" t="s">
         <v>82</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="41">
         <f xml:space="preserve"> 19/21</f>
         <v>0.90476190476190477</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>78</v>
       </c>
@@ -7453,15 +7471,15 @@
       <c r="C14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="37" t="s">
         <v>103</v>
       </c>
-      <c r="F14" s="42">
+      <c r="F14" s="41">
         <f xml:space="preserve"> 15/21</f>
         <v>0.7142857142857143</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>83</v>
       </c>
@@ -7471,16 +7489,17 @@
       <c r="C15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="E15" s="40" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="43">
+      <c r="F15" s="42">
         <f xml:space="preserve"> 20/21</f>
         <v>0.95238095238095233</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <tableParts count="2">
     <tablePart r:id="rId2"/>
@@ -7497,20 +7516,20 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="5" width="32.7265625" customWidth="1"/>
+    <col min="1" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="5" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="44" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="47" t="s">
+      <c r="C1" s="46" t="s">
         <v>102</v>
       </c>
       <c r="D1" s="6" t="s">
@@ -7520,14 +7539,14 @@
         <v>105</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
         <v>31</v>
       </c>
       <c r="B2" s="1">
         <v>7</v>
       </c>
-      <c r="C2" s="44">
+      <c r="C2" s="43">
         <v>12</v>
       </c>
       <c r="D2" s="1" t="s">
@@ -7537,14 +7556,14 @@
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A3" s="37" t="s">
         <v>29</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="44">
+      <c r="C3" s="43">
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -7554,14 +7573,14 @@
         <v>109</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A4" s="41" t="s">
+    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A4" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="48">
+      <c r="B4" s="47">
         <v>10</v>
       </c>
-      <c r="C4" s="49">
+      <c r="C4" s="48">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
@@ -7571,6 +7590,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -7582,34 +7602,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F08444-4000-4A0F-9CD0-9E41C62F8163}">
   <dimension ref="A1:C24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="32.08984375" customWidth="1"/>
-    <col min="3" max="3" width="34.90625" customWidth="1"/>
-    <col min="4" max="4" width="47.6328125" customWidth="1"/>
-    <col min="5" max="6" width="26.1796875" customWidth="1"/>
+    <col min="1" max="2" width="32.1640625" customWidth="1"/>
+    <col min="3" max="3" width="34.83203125" customWidth="1"/>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="6" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="39" t="s">
         <v>9</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A2" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="52">
+      <c r="B2" s="51">
         <f xml:space="preserve"> 18/21</f>
         <v>0.8571428571428571</v>
       </c>
@@ -7617,11 +7637,11 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="38" t="s">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="52">
+      <c r="B3" s="51">
         <f>7/21</f>
         <v>0.33333333333333331</v>
       </c>
@@ -7629,11 +7649,11 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="38" t="s">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="37" t="s">
         <v>110</v>
       </c>
-      <c r="B4" s="52">
+      <c r="B4" s="51">
         <f>10/21</f>
         <v>0.47619047619047616</v>
       </c>
@@ -7641,11 +7661,11 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="53">
+      <c r="B5" s="52">
         <f>8/21</f>
         <v>0.38095238095238093</v>
       </c>
@@ -7653,13 +7673,13 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="16" t="s">
+    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="15" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
@@ -7670,7 +7690,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>6</v>
       </c>
@@ -7681,7 +7701,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -7692,7 +7712,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>46</v>
       </c>
@@ -7703,18 +7723,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="14" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>5</v>
       </c>
@@ -7725,8 +7745,8 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -7736,13 +7756,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="16" t="s">
+    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>10</v>
       </c>
@@ -7753,7 +7773,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>6</v>
       </c>
@@ -7764,7 +7784,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>4</v>
       </c>
@@ -7775,7 +7795,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>46</v>
       </c>
@@ -7786,18 +7806,18 @@
         <v>67</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>5</v>
       </c>
@@ -7808,19 +7828,20 @@
         <v>68</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A24" s="14" t="s">
+    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="16" t="s">
         <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
@@ -7832,208 +7853,208 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BC9C35-D9FF-4137-8E2C-FCA75837906B}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="28.7265625" customWidth="1"/>
+    <col min="1" max="4" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="50" t="s">
+    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="50" t="s">
+      <c r="B1" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="50" t="s">
+      <c r="C1" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="50" t="s">
+      <c r="D1" s="49" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="50" t="s">
+    <row r="2" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="50" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="50" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="50" t="s">
+    <row r="3" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="50" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="51" t="s">
+      <c r="D3" s="50" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="50" t="s">
+    <row r="4" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="49" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="50" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="50" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="50" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="50" t="s">
+    <row r="5" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="49" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="50" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="50" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="50" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="50" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="51" t="s">
+      <c r="D6" s="50" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="50" t="s">
+    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="49" t="s">
         <v>137</v>
       </c>
-      <c r="B7" s="51" t="s">
+      <c r="B7" s="50" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="51" t="s">
+      <c r="C7" s="50" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="51" t="s">
+      <c r="D7" s="50" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="50" t="s">
+    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="49" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="51" t="s">
+      <c r="C8" s="50" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="51" t="s">
+      <c r="D8" s="50" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="50" t="s">
+    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="49" t="s">
         <v>145</v>
       </c>
-      <c r="B9" s="51" t="s">
+      <c r="B9" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="50" t="s">
         <v>147</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="50" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="50" t="s">
+    <row r="10" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="49" t="s">
         <v>149</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="50" t="s">
         <v>150</v>
       </c>
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="50" t="s">
         <v>151</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="50" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="50" t="s">
+    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="49" t="s">
         <v>153</v>
       </c>
-      <c r="B11" s="51" t="s">
+      <c r="B11" s="50" t="s">
         <v>154</v>
       </c>
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="50" t="s">
         <v>155</v>
       </c>
-      <c r="D11" s="51" t="s">
+      <c r="D11" s="50" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="50" t="s">
+    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="49" t="s">
         <v>157</v>
       </c>
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="50" t="s">
         <v>158</v>
       </c>
-      <c r="C12" s="51" t="s">
+      <c r="C12" s="50" t="s">
         <v>159</v>
       </c>
-      <c r="D12" s="51" t="s">
+      <c r="D12" s="50" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="50" t="s">
+    <row r="13" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="49" t="s">
         <v>161</v>
       </c>
-      <c r="B13" s="51" t="s">
+      <c r="B13" s="50" t="s">
         <v>162</v>
       </c>
-      <c r="C13" s="51" t="s">
+      <c r="C13" s="50" t="s">
         <v>163</v>
       </c>
-      <c r="D13" s="51" t="s">
+      <c r="D13" s="50" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="50" t="s">
+    <row r="14" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="50" t="s">
         <v>166</v>
       </c>
-      <c r="C14" s="51" t="s">
+      <c r="C14" s="50" t="s">
         <v>167</v>
       </c>
-      <c r="D14" s="51" t="s">
+      <c r="D14" s="50" t="s">
         <v>168</v>
       </c>
     </row>
@@ -8051,12 +8072,12 @@
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="25.90625" customWidth="1"/>
+    <col min="1" max="7" width="25.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
       <c r="A1" s="9" t="s">
         <v>35</v>
       </c>
@@ -8079,7 +8100,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
         <v>31</v>
       </c>
@@ -8090,7 +8111,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>29</v>
       </c>
@@ -8101,7 +8122,7 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
         <v>27</v>
       </c>
@@ -8112,7 +8133,7 @@
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -8123,8 +8144,8 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="30" t="s">
+    <row r="6" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
         <v>74</v>
       </c>
       <c r="B6" s="4"/>
@@ -8134,8 +8155,8 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="30" t="s">
+    <row r="7" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="29" t="s">
         <v>95</v>
       </c>
       <c r="B7" s="7"/>
@@ -8145,8 +8166,8 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
         <v>96</v>
       </c>
       <c r="B8" s="2"/>
@@ -8158,6 +8179,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -8169,79 +8191,80 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="113.453125" customWidth="1"/>
+    <col min="1" max="1" width="113.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="54" t="s">
+    <row r="2" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="53" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" s="54"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" s="54"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" s="54"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" s="54"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A7" s="54"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A8" s="54"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A9" s="54"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A10" s="54"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A11" s="54"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A12" s="54"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A13" s="54"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A15" s="54"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A16" s="54"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A17" s="54"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A18" s="54"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A19" s="54"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A20" s="54"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="53"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="53"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="53"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="53"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="53"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="53"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="53"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="53"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="53"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="53"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="53"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="53"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="53"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="53"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="53"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="53"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="53"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A2:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Excel erweitert/ aktualsiert
</commit_message>
<xml_diff>
--- a/Excel/Quantitative Analyse.xlsx
+++ b/Excel/Quantitative Analyse.xlsx
@@ -1,29 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nilsarnold/Documents/WIN-Studium/7. Semester/BA/Thesis/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bosch-my.sharepoint.com/personal/nnr3fe_bosch_com/Documents/PersonalDrive/HTWG/BA/LaTex/Thesis/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56C76D2-B746-5A4B-970B-AE29C2E1C97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{E56C76D2-B746-5A4B-970B-AE29C2E1C97D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{319CB7C6-954C-4606-A08A-2E94AF7601B2}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Harmonisierung" sheetId="1" r:id="rId1"/>
-    <sheet name="Jahr" sheetId="8" r:id="rId2"/>
-    <sheet name="Use cases" sheetId="5" r:id="rId3"/>
-    <sheet name="Lernparadigmen" sheetId="10" r:id="rId4"/>
-    <sheet name="KI-Ansatz" sheetId="2" r:id="rId5"/>
-    <sheet name="Zeitplan" sheetId="11" r:id="rId6"/>
-    <sheet name="Kreuztabelle" sheetId="6" r:id="rId7"/>
-    <sheet name="Keywords" sheetId="9" r:id="rId8"/>
+    <sheet name="Jahr" sheetId="8" r:id="rId1"/>
+    <sheet name="Use cases" sheetId="5" r:id="rId2"/>
+    <sheet name="Lernparadigmen" sheetId="10" r:id="rId3"/>
+    <sheet name="Algorithmen" sheetId="2" r:id="rId4"/>
+    <sheet name="Zeitplan" sheetId="11" r:id="rId5"/>
+    <sheet name="Kreuztabelle" sheetId="6" r:id="rId6"/>
+    <sheet name="Keywords" sheetId="9" r:id="rId7"/>
+    <sheet name="Sonstiges" sheetId="12" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Zeitplan!$A$1:$D$14</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Zeitplan!$A$1:$D$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,14 +46,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="158">
   <si>
     <t>5x</t>
   </si>
   <si>
-    <t>Microservices / Serverless</t>
-  </si>
-  <si>
     <t>7x</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>Kubernetes / Orchestrierung</t>
   </si>
   <si>
-    <t>Kubernetes, K8s, Containerization</t>
-  </si>
-  <si>
     <t>Belegte Paper</t>
   </si>
   <si>
@@ -84,75 +78,27 @@
     <t>MLOps Tools (Spezifisch)</t>
   </si>
   <si>
-    <t>Kubeflow, MLFlow, TFX, Ray, Tekton, MLRun</t>
-  </si>
-  <si>
-    <t>Security / DevSecOps</t>
-  </si>
-  <si>
-    <t>Security Scans, Threat Detection, Intrusion Detection, Cybersecurity Risk Modeling</t>
-  </si>
-  <si>
-    <t>Observability, Prometheus, Grafana, AWS CloudWatch, AIOps</t>
-  </si>
-  <si>
     <t>Jahr</t>
   </si>
   <si>
-    <t>Resource Allocation / Scaling</t>
-  </si>
-  <si>
-    <t>Resource Allocation, Dynamic Ressourcenzuweisung, Auto-Scaling</t>
-  </si>
-  <si>
     <t>8x</t>
   </si>
   <si>
-    <t>CI/CD, Build Optimization, Automated Testing, Automated Rollbacks</t>
-  </si>
-  <si>
     <t>Methode/Algorithmus</t>
   </si>
   <si>
-    <t>Generative AI (GenAI)</t>
-  </si>
-  <si>
-    <t>Generative AI, LLMs, ChatGPT, OpenAI CodeX, GitHub Copilot, RAG</t>
-  </si>
-  <si>
     <t>Deep Learning (DL)</t>
   </si>
   <si>
-    <t>Predictive Modeling / Analytics</t>
-  </si>
-  <si>
-    <t>Predictive AI, Predictive Analytics, Predictive Modeling</t>
-  </si>
-  <si>
     <t>Reinforcement Learning (RL)</t>
   </si>
   <si>
-    <t>Reinforcement Modeling, RL, DQN</t>
-  </si>
-  <si>
     <t>Unsupervised Learning (UL)</t>
   </si>
   <si>
-    <t>CNN, RNN, LSTM, BERT, Neural Networks, Deep Learning</t>
-  </si>
-  <si>
     <t>Supervised Learning (SL)</t>
   </si>
   <si>
-    <t>Tree/Ensemble Methods (inkl. RF, DT, XGBoost)</t>
-  </si>
-  <si>
-    <t>Random Forest, RF, Decision Tree, DT, XGBoost, Gradient Boosting</t>
-  </si>
-  <si>
-    <t>Kubernetes / Orchestrierung (inkl. Skalierung)</t>
-  </si>
-  <si>
     <t>KI-Technologie / Lernparadigma</t>
   </si>
   <si>
@@ -162,12 +108,6 @@
     <t>Lernparadigma</t>
   </si>
   <si>
-    <t>Harmonisierte Kategorie</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ursprüngliche Begriffe </t>
-  </si>
-  <si>
     <t>Explizit</t>
   </si>
   <si>
@@ -258,9 +198,6 @@
     <t>P2, P4, P5, P6, P11, P14, P16, P17, P18, P21</t>
   </si>
   <si>
-    <t xml:space="preserve">P1, P3, P4, P10, P11, P12, P13, P14, P16, P17 </t>
-  </si>
-  <si>
     <t>Clustering</t>
   </si>
   <si>
@@ -357,9 +294,6 @@
     <t>Implizit</t>
   </si>
   <si>
-    <t xml:space="preserve">Integrationskomplexität </t>
-  </si>
-  <si>
     <t>Explizit Paper</t>
   </si>
   <si>
@@ -367,12 +301,6 @@
   </si>
   <si>
     <t>P3, P12, P14</t>
-  </si>
-  <si>
-    <t>P3, P4, P6, P11 P12, P14, P18</t>
-  </si>
-  <si>
-    <t>P1, P2, P5,P8, P9, P13, P15,  P16, P17, P19, P20, P21</t>
   </si>
   <si>
     <t>P2, P6, P8, P11, P15, P17, P20, P21</t>
@@ -740,6 +668,45 @@
   </si>
   <si>
     <t xml:space="preserve">BA finalisieren </t>
+  </si>
+  <si>
+    <t>Optimierung von CI/CD-Pipelines</t>
+  </si>
+  <si>
+    <t>Resilienz, Self-Healing und Predictive Maintenance</t>
+  </si>
+  <si>
+    <t>Intelligente Bereitstellung (Edge-AI &amp; Serverless)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AI Governance, Datenschutz und Compliance </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Integrationskomplexität &amp; Abhängigkeiten </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Datenqualität, Datenverfügbarkeit und Heterogenität </t>
+  </si>
+  <si>
+    <t>P1, P2, P5,P8, P9, P13, P15,  P16, P17, P20, P21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Erwähnt </t>
+  </si>
+  <si>
+    <t>Erwähnt</t>
+  </si>
+  <si>
+    <t>P11, P19</t>
+  </si>
+  <si>
+    <t>P3, P4, P6, P12, P14, P18</t>
+  </si>
+  <si>
+    <t>P1, P4, P13, P16</t>
+  </si>
+  <si>
+    <t>P3, P10, P11, P12, P14, P17, P19</t>
   </si>
 </sst>
 </file>
@@ -807,15 +774,21 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -949,12 +922,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1064,24 +1076,6 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1094,15 +1088,202 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="35">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1228,8 +1409,54 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
-        <b val="0"/>
+        <b/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1246,157 +1473,10 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
+        <left style="medium">
           <color indexed="64"/>
         </left>
         <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color auto="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
@@ -1910,7 +1990,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2045,9 +2125,6 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -2286,7 +2363,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2294,6 +2370,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2457,7 +2534,7 @@
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>CI/CD Automatisierung &amp; Pipeline-Optimierung</c:v>
+                  <c:v>Optimierung von CI/CD-Pipelines</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Ressourcen- &amp; Workload-Optimierung</c:v>
@@ -2466,10 +2543,10 @@
                   <c:v>Sicherheits- &amp; Bedrohungserkennung</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Automatische Fehlererkennung &amp; Systemstabilität</c:v>
+                  <c:v>Resilienz, Self-Healing und Predictive Maintenance</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Verteilte oder leichtgewichtige Umgebungen (Serveless Deployment) </c:v>
+                  <c:v>Intelligente Bereitstellung (Edge-AI &amp; Serverless)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2484,16 +2561,16 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>3</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>2</c:v>
-                </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2632,7 +2709,6 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -2640,6 +2716,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2792,13 +2869,13 @@
                   <c:v>Skalierbarkeit, Latenz &amp; Monitoring</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>AI Governance &amp; Security </c:v>
+                  <c:v>AI Governance, Datenschutz und Compliance </c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Integrationskomplexität </c:v>
+                  <c:v>Integrationskomplexität &amp; Abhängigkeiten </c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Datenmanagement &amp; Qualität </c:v>
+                  <c:v>Datenqualität, Datenverfügbarkeit und Heterogenität </c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2810,19 +2887,19 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>0.95238095238095233</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.90476190476190477</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.90476190476190477</c:v>
+                  <c:v>0.80952380952380953</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>0.80952380952380953</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.7142857142857143</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.95238095238095233</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3011,6 +3088,316 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Use cases'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Häufigkeit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-3501-4B2E-91D3-558D5FBFB45B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000003-3501-4B2E-91D3-558D5FBFB45B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="2"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000005-3501-4B2E-91D3-558D5FBFB45B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="3"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000007-3501-4B2E-91D3-558D5FBFB45B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="19050">
+                <a:solidFill>
+                  <a:schemeClr val="lt1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000009-3501-4B2E-91D3-558D5FBFB45B}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Use cases'!$E$2:$E$6</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>Optimierung von CI/CD-Pipelines</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Ressourcen- &amp; Workload-Optimierung</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Sicherheits- &amp; Bedrohungserkennung</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Resilienz, Self-Healing und Predictive Maintenance</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Intelligente Bereitstellung (Edge-AI &amp; Serverless)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Use cases'!$F$2:$F$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C99D-4969-B71A-FB59B7DCCFD6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -3143,13 +3530,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3208,7 +3595,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>8</c:v>
@@ -3222,6 +3609,71 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-280F-440F-95BF-9EB6C8338D88}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Lernparadigmen!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Erwähnt </c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Lernparadigmen!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Supervised Learning (SL)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Unsupervised Learning (UL)</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Reinforcement Learning (RL)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Lernparadigmen!$D$2:$D$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-89F6-45B9-8306-CA89A9B14D1D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -3380,7 +3832,6 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -3388,6 +3839,7 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -3422,7 +3874,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="de-DE"/>
@@ -3520,7 +3972,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'KI-Ansatz'!$B$1</c:f>
+              <c:f>Algorithmen!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3541,7 +3993,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>'KI-Ansatz'!$A$2:$A$5</c:f>
+              <c:f>Algorithmen!$A$2:$A$5</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -3561,7 +4013,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'KI-Ansatz'!$B$2:$B$5</c:f>
+              <c:f>Algorithmen!$B$2:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="4"/>
@@ -3572,10 +4024,10 @@
                   <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.47619047619047616</c:v>
+                  <c:v>0.52380952380952384</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38095238095238093</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3948,6 +4400,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -5464,7 +5956,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="251">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5521,7 +6013,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -5572,6 +6064,13 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5582,12 +6081,19 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
@@ -5625,6 +6131,511 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
     <cs:fillRef idx="1"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
@@ -5966,7 +6977,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6584,6 +7595,42 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>50427</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>82736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>50427</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>77320</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1C1E7A1-BC01-2620-A179-CB01DACE4CEF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -6597,7 +7644,7 @@
       <xdr:rowOff>11112</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>2132012</xdr:colOff>
       <xdr:row>21</xdr:row>
       <xdr:rowOff>46037</xdr:rowOff>
@@ -6632,16 +7679,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>801158</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>303741</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>727075</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>49741</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>222250</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>157691</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>811742</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>97366</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6670,59 +7717,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9CC33F1-D254-49F3-8557-E5C7872583BF}" name="Tabelle1" displayName="Tabelle1" ref="A1:E6" totalsRowShown="0" headerRowDxfId="32" headerRowBorderDxfId="31" tableBorderDxfId="30" totalsRowBorderDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B9CC33F1-D254-49F3-8557-E5C7872583BF}" name="Tabelle1" displayName="Tabelle1" ref="A1:E6" totalsRowShown="0" headerRowDxfId="34" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
   <autoFilter ref="A1:E6" xr:uid="{B9CC33F1-D254-49F3-8557-E5C7872583BF}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{620D4100-10BB-4135-B53B-6B5034AFE668}" name="Jahr" dataDxfId="28"/>
-    <tableColumn id="2" xr3:uid="{D134C25B-4B6A-4AAB-AF1C-8A8225861C02}" name="Journal" dataDxfId="27"/>
-    <tableColumn id="3" xr3:uid="{10A7D4DA-004F-4919-AD06-7AB2A5AA9262}" name="Conference" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{EA1054E4-076B-47F9-9C72-0D8023C3392B}" name="Arxiv" dataDxfId="25"/>
-    <tableColumn id="5" xr3:uid="{DDFEFE86-2761-4404-8068-121B7CDC91D0}" name="Whitepaper" dataDxfId="24"/>
+    <tableColumn id="1" xr3:uid="{620D4100-10BB-4135-B53B-6B5034AFE668}" name="Jahr" dataDxfId="30"/>
+    <tableColumn id="2" xr3:uid="{D134C25B-4B6A-4AAB-AF1C-8A8225861C02}" name="Journal" dataDxfId="29"/>
+    <tableColumn id="3" xr3:uid="{10A7D4DA-004F-4919-AD06-7AB2A5AA9262}" name="Conference" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{EA1054E4-076B-47F9-9C72-0D8023C3392B}" name="Arxiv" dataDxfId="27"/>
+    <tableColumn id="5" xr3:uid="{DDFEFE86-2761-4404-8068-121B7CDC91D0}" name="Whitepaper" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{278AE58D-B189-4269-A605-97111FBD9467}" name="Tabelle2" displayName="Tabelle2" ref="E1:F6" totalsRowShown="0" headerRowDxfId="23" headerRowBorderDxfId="22" tableBorderDxfId="21" totalsRowBorderDxfId="20">
-  <autoFilter ref="E1:F6" xr:uid="{278AE58D-B189-4269-A605-97111FBD9467}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B517C7E9-96D7-4177-BCC7-4D8BF4066876}" name="Tabelle27" displayName="Tabelle27" ref="E1:F6" totalsRowShown="0" headerRowDxfId="25" headerRowBorderDxfId="24" tableBorderDxfId="23" totalsRowBorderDxfId="22">
+  <autoFilter ref="E1:F6" xr:uid="{B517C7E9-96D7-4177-BCC7-4D8BF4066876}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{A5ECC236-9CC3-40B6-9A99-74F580ABEC55}" name="Use Case" dataDxfId="19"/>
-    <tableColumn id="2" xr3:uid="{BA5D8B57-4B50-440C-9933-C8305A23CF91}" name="Häufigkeit" dataDxfId="18"/>
+    <tableColumn id="1" xr3:uid="{FA5B63D2-4D69-40B0-A8C4-99534F932421}" name="Use Case" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{22E39CEE-4C36-4391-9DC9-B26D6BB1FBFA}" name="Häufigkeit" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1B9BB0B9-4763-4189-A791-B09190FEC97A}" name="Tabelle3" displayName="Tabelle3" ref="E10:F15" totalsRowShown="0" headerRowDxfId="17" headerRowBorderDxfId="16" tableBorderDxfId="15" totalsRowBorderDxfId="14">
-  <autoFilter ref="E10:F15" xr:uid="{1B9BB0B9-4763-4189-A791-B09190FEC97A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D4EAD1EC-A7FE-4C98-8156-9219E942A8BE}" name="Tabelle38" displayName="Tabelle38" ref="E10:F15" totalsRowShown="0" headerRowDxfId="19" headerRowBorderDxfId="18" tableBorderDxfId="17" totalsRowBorderDxfId="16">
+  <autoFilter ref="E10:F15" xr:uid="{D4EAD1EC-A7FE-4C98-8156-9219E942A8BE}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{8B774025-867F-4AA1-9B98-EF89FAACDAE3}" name="Herausforderung" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{DACDBAA5-4CAF-441E-81BC-77C2C782EBEB}" name="Häufigkeit" dataDxfId="12" dataCellStyle="Prozent"/>
+    <tableColumn id="1" xr3:uid="{D4C53F4C-670A-4398-9895-7693BEFE023D}" name="Herausforderung" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{88D328E2-D6AF-4CA3-8BCE-7BF47C182462}" name="Häufigkeit" dataDxfId="14" dataCellStyle="Prozent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A62E4DE7-B15D-4164-9E48-FA7C94CE72C0}" name="Tabelle4" displayName="Tabelle4" ref="A1:C4" totalsRowShown="0" headerRowBorderDxfId="11" tableBorderDxfId="10" totalsRowBorderDxfId="9">
-  <autoFilter ref="A1:C4" xr:uid="{A62E4DE7-B15D-4164-9E48-FA7C94CE72C0}"/>
-  <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{F14AF351-14AF-44A5-8947-E212E1F47F29}" name="Lernparadigma" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{3A7749C9-6DF4-43D7-B809-334A1DA17A06}" name="Explizit" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{FD12B577-2D81-43CF-8D4F-FB76FE8141A1}" name="Implizit" dataDxfId="6"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{A62E4DE7-B15D-4164-9E48-FA7C94CE72C0}" name="Tabelle4" displayName="Tabelle4" ref="A1:D4" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="13" tableBorderDxfId="12" totalsRowBorderDxfId="11">
+  <autoFilter ref="A1:D4" xr:uid="{A62E4DE7-B15D-4164-9E48-FA7C94CE72C0}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{F14AF351-14AF-44A5-8947-E212E1F47F29}" name="Lernparadigma" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{3A7749C9-6DF4-43D7-B809-334A1DA17A06}" name="Explizit" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{FD12B577-2D81-43CF-8D4F-FB76FE8141A1}" name="Implizit" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{4C2CAFC5-567F-4E51-86AE-A38E907606CB}" name="Erwähnt " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A642C74E-4190-462E-BAF0-66E01C41D1AC}" name="Tabelle5" displayName="Tabelle5" ref="A1:B5" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3" totalsRowBorderDxfId="2">
-  <autoFilter ref="A1:B5" xr:uid="{A642C74E-4190-462E-BAF0-66E01C41D1AC}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{997ABBB2-BD81-4BB5-B021-45BB4E97412D}" name="Tabelle59" displayName="Tabelle59" ref="A1:B5" totalsRowShown="0" headerRowDxfId="10" headerRowBorderDxfId="9" tableBorderDxfId="8" totalsRowBorderDxfId="7">
+  <autoFilter ref="A1:B5" xr:uid="{997ABBB2-BD81-4BB5-B021-45BB4E97412D}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{22D3E909-73E1-40FC-A71B-150952C70172}" name="Methode/Algorithmus" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{8DDB1D05-7A6A-4DE9-A063-97C2044254E3}" name="Häufigkeit" dataDxfId="0" dataCellStyle="Prozent"/>
+    <tableColumn id="1" xr3:uid="{BC3A2AA9-E3FB-4C23-98FB-3C9ECCB4D228}" name="Methode/Algorithmus" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{F0E647BA-D317-4092-96EF-C9BC7AF21C97}" name="Häufigkeit" dataDxfId="5" dataCellStyle="Prozent"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -6990,511 +8038,392 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2226A24-3CB1-4FB4-B481-A184711D649A}">
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="52.33203125" customWidth="1"/>
-    <col min="2" max="2" width="56.1640625" customWidth="1"/>
-    <col min="3" max="27" width="29.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="2" max="3" width="21.453125" customWidth="1"/>
+    <col min="4" max="4" width="25.1796875" customWidth="1"/>
+    <col min="5" max="5" width="27.6328125" customWidth="1"/>
+    <col min="6" max="7" width="21.453125" customWidth="1"/>
+    <col min="8" max="8" width="27.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="E1" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="F1" s="19"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="20">
+        <v>2021</v>
+      </c>
+      <c r="B2" s="18">
+        <v>2</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="21"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="20">
+        <v>2022</v>
+      </c>
+      <c r="B3" s="18">
+        <v>1</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="21"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="20">
+        <v>2023</v>
+      </c>
+      <c r="B4" s="18">
+        <v>2</v>
+      </c>
+      <c r="C4" s="18"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="21"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="20">
+        <v>2024</v>
+      </c>
+      <c r="B5" s="18">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" ht="32" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
+      <c r="C5" s="18">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="25">
+        <v>2025</v>
+      </c>
+      <c r="B6" s="26">
         <v>7</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
+      <c r="C6" s="26">
+        <v>1</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="E6" s="28"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="17"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="17"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2226A24-3CB1-4FB4-B481-A184711D649A}">
-  <dimension ref="A1:F17"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" sqref="A1:E6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="16.83203125" customWidth="1"/>
-    <col min="2" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" customWidth="1"/>
-    <col min="5" max="5" width="27.6640625" customWidth="1"/>
-    <col min="6" max="7" width="21.5" customWidth="1"/>
-    <col min="8" max="8" width="27.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="B1" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="E1" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="19"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="20">
-        <v>2021</v>
-      </c>
-      <c r="B2" s="18">
-        <v>2</v>
-      </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="21"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="20">
-        <v>2022</v>
-      </c>
-      <c r="B3" s="18">
-        <v>1</v>
-      </c>
-      <c r="C3" s="18"/>
-      <c r="D3" s="16"/>
-      <c r="E3" s="21"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="20">
-        <v>2023</v>
-      </c>
-      <c r="B4" s="18">
-        <v>2</v>
-      </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="21"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="20">
-        <v>2024</v>
-      </c>
-      <c r="B5" s="18">
-        <v>5</v>
-      </c>
-      <c r="C5" s="18">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" s="25">
-        <v>2025</v>
-      </c>
-      <c r="B6" s="26">
-        <v>6</v>
-      </c>
-      <c r="C6" s="26">
-        <v>1</v>
-      </c>
-      <c r="D6" s="27">
-        <v>1</v>
-      </c>
-      <c r="E6" s="28"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="17"/>
-      <c r="C7" s="17"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" s="17"/>
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14" s="17"/>
-      <c r="B14" s="17"/>
-      <c r="C14" s="17"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15" s="17"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24799D05-FC12-4E10-8DB7-F9A31CAD1DF2}">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.33203125" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
-    <col min="3" max="3" width="37.83203125" customWidth="1"/>
-    <col min="5" max="6" width="23.1640625" style="30" customWidth="1"/>
+    <col min="1" max="1" width="31.36328125" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="3" max="3" width="37.81640625" customWidth="1"/>
+    <col min="5" max="6" width="23.1796875" style="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="33" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="F1" s="34" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="12" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="E2" s="31" t="s">
-        <v>41</v>
+        <v>145</v>
       </c>
       <c r="F2" s="32">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="12" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B3" s="13" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="E3" s="31" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="F3" s="32">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="E4" s="31" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="F4" s="32">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E5" s="31" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" s="32">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" s="12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="E5" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="F5" s="32">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="12" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C6" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="E6" s="35" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="36">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="B10" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="E10" s="38" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="F10" s="39" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="C11" s="2"/>
-      <c r="E11" s="37" t="s">
-        <v>80</v>
+      <c r="E11" s="49" t="s">
+        <v>59</v>
       </c>
       <c r="F11" s="41">
-        <f xml:space="preserve"> 21/21</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> 20/21</f>
+        <v>0.95238095238095233</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="E12" s="37" t="s">
-        <v>81</v>
+        <v>63</v>
+      </c>
+      <c r="E12" s="50" t="s">
+        <v>60</v>
       </c>
       <c r="F12" s="41">
         <f xml:space="preserve"> 19/21</f>
         <v>0.90476190476190477</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="E13" s="37" t="s">
-        <v>82</v>
+        <v>66</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>148</v>
       </c>
       <c r="F13" s="41">
-        <f xml:space="preserve"> 19/21</f>
-        <v>0.90476190476190477</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+        <f xml:space="preserve"> 17/21</f>
+        <v>0.80952380952380953</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E14" s="37" t="s">
-        <v>103</v>
+        <v>67</v>
+      </c>
+      <c r="E14" s="50" t="s">
+        <v>149</v>
       </c>
       <c r="F14" s="41">
+        <f xml:space="preserve"> 17/21</f>
+        <v>0.80952380952380953</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" s="51" t="s">
+        <v>150</v>
+      </c>
+      <c r="F15" s="42">
         <f xml:space="preserve"> 15/21</f>
         <v>0.7142857142857143</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="32" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>83</v>
-      </c>
-      <c r="F15" s="42">
-        <f xml:space="preserve"> 20/21</f>
-        <v>0.95238095238095233</v>
       </c>
     </row>
   </sheetData>
@@ -7508,554 +8437,411 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B6F798B-F129-4C52-8944-FD82D34941C3}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="17.83203125" customWidth="1"/>
-    <col min="4" max="5" width="32.6640625" customWidth="1"/>
+    <col min="1" max="4" width="17.81640625" customWidth="1"/>
+    <col min="5" max="6" width="32.6328125" customWidth="1"/>
+    <col min="7" max="7" width="19.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="44" t="s">
-        <v>37</v>
-      </c>
-      <c r="B1" s="45" t="s">
-        <v>40</v>
-      </c>
-      <c r="C1" s="46" t="s">
-        <v>102</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>104</v>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="53" t="s">
+        <v>81</v>
+      </c>
+      <c r="D1" s="54" t="s">
+        <v>152</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
-        <v>31</v>
+        <v>82</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="1">
-        <v>7</v>
-      </c>
-      <c r="C2" s="43">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>107</v>
+        <v>6</v>
+      </c>
+      <c r="C2" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
+        <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
-        <v>29</v>
+        <v>155</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>3</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="1">
         <v>8</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>106</v>
+      <c r="D3" s="1">
+        <v>0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A4" s="40" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="47">
-        <v>10</v>
-      </c>
-      <c r="C4" s="48">
+        <v>84</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E4" s="1"/>
+      <c r="D4" s="1">
+        <v>4</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="2" t="s">
+        <v>156</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F08444-4000-4A0F-9CD0-9E41C62F8163}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection sqref="A1:B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="32.1796875" customWidth="1"/>
+    <col min="3" max="3" width="34.81640625" customWidth="1"/>
+    <col min="4" max="4" width="47.6328125" customWidth="1"/>
+    <col min="5" max="6" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="45">
+        <f xml:space="preserve"> 18/21</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="45">
+        <f>7/21</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="37" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="45">
+        <f>11/21</f>
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="46">
+        <f>7/21</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9F08444-4000-4A0F-9CD0-9E41C62F8163}">
-  <dimension ref="A1:C24"/>
-  <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="2" width="32.1640625" customWidth="1"/>
-    <col min="3" max="3" width="34.83203125" customWidth="1"/>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
-    <col min="5" max="6" width="26.1640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="39" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
-        <v>73</v>
-      </c>
-      <c r="B2" s="51">
-        <f xml:space="preserve"> 18/21</f>
-        <v>0.8571428571428571</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="B3" s="51">
-        <f>7/21</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
-        <v>110</v>
-      </c>
-      <c r="B4" s="51">
-        <f>10/21</f>
-        <v>0.47619047619047616</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="40" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="52">
-        <f>8/21</f>
-        <v>0.38095238095238093</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="10"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="32" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C24" s="16" t="s">
-        <v>69</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-  <drawing r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4BC9C35-D9FF-4137-8E2C-FCA75837906B}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="28.6640625" customWidth="1"/>
+    <col min="1" max="4" width="28.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49" t="s">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="B1" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="C1" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="D1" s="43" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="43" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="44" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>103</v>
+      </c>
+      <c r="D4" s="44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="43" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" s="44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C6" s="44" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" s="44" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="49" t="s">
+      <c r="B7" s="44" t="s">
         <v>114</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C7" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="D1" s="49" t="s">
+      <c r="D7" s="44" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+    <row r="8" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B8" s="44" t="s">
         <v>118</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C8" s="44" t="s">
         <v>119</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D8" s="44" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="49" t="s">
+    <row r="9" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="50" t="s">
+      <c r="B9" s="44" t="s">
         <v>122</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C9" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="D3" s="50" t="s">
+      <c r="D9" s="44" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="49" t="s">
+    <row r="10" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B10" s="44" t="s">
         <v>126</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C10" s="44" t="s">
         <v>127</v>
       </c>
-      <c r="D4" s="50" t="s">
+      <c r="D10" s="44" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="43" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="B11" s="44" t="s">
         <v>130</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C11" s="44" t="s">
         <v>131</v>
       </c>
-      <c r="D5" s="50" t="s">
+      <c r="D11" s="44" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+    <row r="12" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="43" t="s">
         <v>133</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="B12" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="C6" s="50" t="s">
+      <c r="C12" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="D6" s="50" t="s">
+      <c r="D12" s="44" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+    <row r="13" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="B7" s="50" t="s">
+      <c r="B13" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="C7" s="50" t="s">
+      <c r="C13" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="D7" s="50" t="s">
+      <c r="D13" s="44" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+    <row r="14" spans="1:4" ht="28.5" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="43" t="s">
         <v>141</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B14" s="44" t="s">
         <v>142</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C14" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="D8" s="50" t="s">
+      <c r="D14" s="44" t="s">
         <v>144</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
-        <v>145</v>
-      </c>
-      <c r="B9" s="50" t="s">
-        <v>146</v>
-      </c>
-      <c r="C9" s="50" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" s="50" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
-        <v>149</v>
-      </c>
-      <c r="B10" s="50" t="s">
-        <v>150</v>
-      </c>
-      <c r="C10" s="50" t="s">
-        <v>151</v>
-      </c>
-      <c r="D10" s="50" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
-        <v>153</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>154</v>
-      </c>
-      <c r="C11" s="50" t="s">
-        <v>155</v>
-      </c>
-      <c r="D11" s="50" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
-        <v>157</v>
-      </c>
-      <c r="B12" s="50" t="s">
-        <v>158</v>
-      </c>
-      <c r="C12" s="50" t="s">
-        <v>159</v>
-      </c>
-      <c r="D12" s="50" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="49" t="s">
-        <v>161</v>
-      </c>
-      <c r="B13" s="50" t="s">
-        <v>162</v>
-      </c>
-      <c r="C13" s="50" t="s">
-        <v>163</v>
-      </c>
-      <c r="D13" s="50" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="49" t="s">
-        <v>165</v>
-      </c>
-      <c r="B14" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="C14" s="50" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="50" t="s">
-        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -8064,89 +8850,83 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0034EA90-740B-4B82-80F7-079B70741AD0}">
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="25.83203125" customWidth="1"/>
+    <col min="1" max="7" width="25.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="G1" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+        <v>17</v>
+      </c>
+      <c r="B1" s="47" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="47" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="9"/>
+    </row>
+    <row r="2" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="4"/>
+        <v>16</v>
+      </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="4"/>
+        <v>15</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="4"/>
+        <v>14</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="4"/>
+        <v>13</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -8155,9 +8935,9 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row r="7" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="29" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -8166,9 +8946,9 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="29" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -8183,7 +8963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DC547C4-CBCF-401F-8D40-69E42280EAE6}">
   <dimension ref="A1:A20"/>
   <sheetViews>
@@ -8191,74 +8971,74 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="113.5" customWidth="1"/>
+    <col min="1" max="1" width="113.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="53" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="53"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="53"/>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="53"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="53"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="53"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="53"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="53"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="53"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="53"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="53"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="53"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="53"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="53"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="53"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="53"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="53"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="53"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="52" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="52"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="52"/>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A5" s="52"/>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="52"/>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="52"/>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" s="52"/>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" s="52"/>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" s="52"/>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" s="52"/>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" s="52"/>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" s="52"/>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" s="52"/>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" s="52"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="52"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" s="52"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" s="52"/>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" s="52"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" s="52"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -8267,4 +9047,188 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F06C7F0-C4EB-46B5-ACB8-905A687213FC}">
+  <dimension ref="A1:C17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="3" width="37.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="10"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>